<commit_message>
new response format xslx:
- added new response parameter for xlsx: sheet_idx
- used to marshall a specific sheet of the xlsx file

see #77805
</commit_message>
<xml_diff>
--- a/test/response/format/xlsx/sample.xlsx
+++ b/test/response/format/xlsx/sample.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="page 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="page 2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">_system_object_id</t>
   </si>
@@ -80,6 +81,27 @@
   </si>
   <si>
     <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview</t>
   </si>
 </sst>
 </file>
@@ -89,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -115,6 +137,14 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -162,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,6 +207,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -198,7 +232,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -206,7 +240,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.58"/>
@@ -584,4 +618,61 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.78125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>